<commit_message>
Add output folder of final tables and figures
</commit_message>
<xml_diff>
--- a/output/tables/DE_comm_detection.xlsx
+++ b/output/tables/DE_comm_detection.xlsx
@@ -444,7 +444,7 @@
         <v>0.4068826337865163</v>
       </c>
       <c r="H2">
-        <v>0.420776999771986</v>
+        <v>0.4207769997719861</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -568,7 +568,7 @@
         <v>3</v>
       </c>
       <c r="F7">
-        <v>1.1503678214196</v>
+        <v>1.150367821419599</v>
       </c>
       <c r="G7">
         <v>0.9411764705882353</v>
@@ -594,7 +594,7 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>0.843609191245676</v>
+        <v>0.8436091912456761</v>
       </c>
       <c r="G8">
         <v>0.7142857142857143</v>
@@ -620,7 +620,7 @@
         <v>4</v>
       </c>
       <c r="F9">
-        <v>0.9925916287340275</v>
+        <v>0.9925916287340277</v>
       </c>
       <c r="G9">
         <v>0.8057965589027999</v>

</xml_diff>